<commit_message>
Fixed excel no row test
</commit_message>
<xml_diff>
--- a/src/test/resources/test10.xlsx
+++ b/src/test/resources/test10.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo245303\Desktop\asw\citloader\citizensLoader_i3b\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17625" windowHeight="7065"/>
   </bookViews>
@@ -10,11 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -71,12 +72,15 @@
   </si>
   <si>
     <t>pollingStation</t>
+  </si>
+  <si>
+    <t>90500081Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,39 +475,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>31330</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>

</xml_diff>